<commit_message>
Update Sprint Backlog 3ºSprint.xlsx
</commit_message>
<xml_diff>
--- a/Sprint Backlog 3ºSprint.xlsx
+++ b/Sprint Backlog 3ºSprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\upskill_java1_labprg_grupo3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A79CFD-4D7F-4109-973A-63E048365BA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A010CC8F-3313-47EB-B1FC-599951603BCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="0" windowWidth="15075" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>Tarefa</t>
   </si>
@@ -54,6 +54,90 @@
   </si>
   <si>
     <t>Base Dados</t>
+  </si>
+  <si>
+    <t>SQL Plataforma</t>
+  </si>
+  <si>
+    <t>SQL Organizacao</t>
+  </si>
+  <si>
+    <t>SQL Administrativo</t>
+  </si>
+  <si>
+    <t>SQL Colaborador</t>
+  </si>
+  <si>
+    <t>SQL Freelancer</t>
+  </si>
+  <si>
+    <t>SQL HabilitacaoAcademica</t>
+  </si>
+  <si>
+    <t>SQL ReconhecimentoCT</t>
+  </si>
+  <si>
+    <t>SQL Utilizador</t>
+  </si>
+  <si>
+    <t>SQL Role</t>
+  </si>
+  <si>
+    <t>SQL CategoriaTarefa</t>
+  </si>
+  <si>
+    <t>SQL Tarefa</t>
+  </si>
+  <si>
+    <t>SQL 
+CaraterizacaoCategoriaTarefa</t>
+  </si>
+  <si>
+    <t>SQL EstadoTarefa</t>
+  </si>
+  <si>
+    <t>SQL Anuncio</t>
+  </si>
+  <si>
+    <t>SQL Candidatura</t>
+  </si>
+  <si>
+    <t>SQL ProcessoSeriacao</t>
+  </si>
+  <si>
+    <t>SQL Classificacao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL 
+ProcessoSeriacaoColaborador
+</t>
+  </si>
+  <si>
+    <t>SQL TipoRegimento</t>
+  </si>
+  <si>
+    <t>SQL CompetenciaTecnica</t>
+  </si>
+  <si>
+    <t>SQL GrauProficiencia</t>
+  </si>
+  <si>
+    <t>SQL AreaAtividade</t>
+  </si>
+  <si>
+    <t>SQL EnderecoPostal</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Julio</t>
+  </si>
+  <si>
+    <t>Vitor</t>
+  </si>
+  <si>
+    <t>Anibal</t>
   </si>
 </sst>
 </file>
@@ -76,7 +160,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -113,7 +196,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -124,19 +207,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -182,19 +252,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -206,7 +284,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -487,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:O235"/>
+  <dimension ref="B3:O235"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -501,554 +591,739 @@
     <col min="6" max="6" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:15" ht="21.75" customHeight="1">
-      <c r="B4" s="1" t="s">
+    <row r="3" spans="2:15" ht="15.75" thickBot="1"/>
+    <row r="4" spans="2:15" ht="21.75" customHeight="1" thickBot="1">
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="40.5" customHeight="1">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="C5" s="3">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" spans="2:15" ht="40.5" customHeight="1">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4">
-        <v>3</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
     </row>
     <row r="7" spans="2:15" ht="40.5" customHeight="1">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4">
-        <v>3</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
     </row>
     <row r="8" spans="2:15" ht="40.5" customHeight="1">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="B8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="2:15" ht="40.5" customHeight="1">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
+      <c r="B9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
     </row>
     <row r="10" spans="2:15" ht="40.5" customHeight="1">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
+      <c r="B10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
     </row>
     <row r="11" spans="2:15" ht="40.5" customHeight="1">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
+      <c r="B11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
     </row>
     <row r="12" spans="2:15" ht="40.5" customHeight="1">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="B12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
     </row>
     <row r="13" spans="2:15" ht="40.5" customHeight="1">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
+      <c r="B13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
     </row>
     <row r="14" spans="2:15" ht="40.5" customHeight="1">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
+      <c r="B14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3">
+        <v>4</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
     </row>
     <row r="15" spans="2:15" ht="40.5" customHeight="1">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
+      <c r="B15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
     </row>
     <row r="16" spans="2:15" ht="40.5" customHeight="1">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="B16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="B17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="18" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="B18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="3">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="B19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="B20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="B21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="3">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="B22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="3">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="23" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="B23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="3">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="24" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="B24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="3">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="25" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="B25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="3">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="26" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="B26" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="3">
+        <v>3</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="27" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="B27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="28" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="B28" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="3">
+        <v>3</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="29" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="B29" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="3">
+        <v>3</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="30" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B30" s="7"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="B30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="31" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B31" s="7"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B32" s="7"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B33" s="7"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B34" s="7"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B35" s="7"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B36" s="6"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B37" s="6"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B38" s="8"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
     </row>
     <row r="39" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B39" s="8"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
     </row>
     <row r="40" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B40" s="8"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
     </row>
     <row r="41" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
     </row>
     <row r="43" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
     </row>
     <row r="50" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
     </row>
     <row r="53" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
     </row>
     <row r="54" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
     </row>
     <row r="55" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
     </row>
     <row r="56" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
     </row>
     <row r="57" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
     </row>
     <row r="58" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
     </row>
     <row r="59" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
     </row>
     <row r="60" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
     </row>
     <row r="61" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
     </row>
     <row r="62" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
     </row>
     <row r="63" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
     </row>
     <row r="64" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
     </row>
     <row r="65" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
     </row>
     <row r="66" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
     </row>
     <row r="67" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
     </row>
     <row r="68" spans="2:6" ht="44.25" customHeight="1">
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
     </row>
     <row r="69" spans="2:6" ht="44.25" customHeight="1">
-      <c r="D69" s="4"/>
+      <c r="D69" s="3"/>
     </row>
     <row r="70" spans="2:6" ht="44.25" customHeight="1">
-      <c r="D70" s="4"/>
+      <c r="D70" s="3"/>
     </row>
     <row r="71" spans="2:6" ht="44.25" customHeight="1"/>
     <row r="72" spans="2:6" ht="44.25" customHeight="1"/>

</xml_diff>